<commit_message>
Change expected xlsx files
</commit_message>
<xml_diff>
--- a/test/functional/xlsx_files/chart_area01.xlsx
+++ b/test/functional/xlsx_files/chart_area01.xlsx
@@ -167,25 +167,35 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="50010003"/>
-        <c:axId val="50010004"/>
+        <c:axId val="43407616"/>
+        <c:axId val="43433984"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="50010003"/>
+        <c:axId val="43407616"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010004"/>
+        <c:crossAx val="43433984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50010004"/>
+        <c:axId val="43433984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -193,7 +203,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010003"/>
+        <c:crossAx val="43407616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>

</xml_diff>